<commit_message>
Excel Adv - Add password option
</commit_message>
<xml_diff>
--- a/argoslabs/data/excel/tests/data_sheet_02.xlsx
+++ b/argoslabs/data/excel/tests/data_sheet_02.xlsx
@@ -17,9 +17,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0\ \ &quot;c/s&quot;"/>
     <numFmt numFmtId="165" formatCode="m&quot;月&quot;d&quot;日&quot;\(aaa\)"/>
+    <numFmt numFmtId="166" formatCode="0&quot;ケース&quot;"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -921,7 +922,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1375,6 +1376,15 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="23" fillId="0" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
@@ -18338,9 +18348,18 @@
       <c r="J1399" s="102" t="n"/>
     </row>
     <row r="1400" ht="18" customHeight="1" s="101">
-      <c r="A1400" s="12" t="n"/>
-      <c r="B1400" s="103" t="n"/>
-      <c r="C1400" s="104" t="n"/>
+      <c r="A1400" s="157">
+        <f>SUMIFS(INDIRECT("data!$FA:$FA"),INDIRECT("data!$Y:$Y"),"9606",INDIRECT("data!$DE:$DE"),$B12)</f>
+        <v/>
+      </c>
+      <c r="B1400" s="158">
+        <f>SUMIFS(INDIRECT("data!$FA:$FA"),INDIRECT("data!$Y:$Y"),"9610",INDIRECT("data!$DE:$DE"),$B12)</f>
+        <v/>
+      </c>
+      <c r="C1400" s="159">
+        <f>SUMIFS(INDIRECT("data!$FA:$FA"),INDIRECT("data!$Y:$Y"),"9611",INDIRECT("data!$DE:$DE"),$B12)</f>
+        <v/>
+      </c>
       <c r="D1400" s="120">
         <f>SUMIFS(INDIRECT("data!$FA:$FA"),INDIRECT("data!$Y:$Y"),"9606",INDIRECT("data!$DE:$DE"),$B12)</f>
         <v/>

</xml_diff>